<commit_message>
fixed issues in multilingual labels cleanup up Readme added previous and next buttons to the learning stage.
</commit_message>
<xml_diff>
--- a/data/servo_mestre.xlsx
+++ b/data/servo_mestre.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>Identifier</t>
   </si>
@@ -29,6 +29,24 @@
   </si>
   <si>
     <t>Fr</t>
+  </si>
+  <si>
+    <t>ButtonNext</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>次</t>
+  </si>
+  <si>
+    <t>ButtonPrevious</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>前</t>
   </si>
   <si>
     <t>Resovoir</t>
@@ -528,29 +546,29 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -562,29 +580,29 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -727,10 +745,10 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -758,41 +776,41 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
@@ -800,29 +818,29 @@
       <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -1203,10 +1221,10 @@
         <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1233,9 +1251,15 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1261,9 +1285,15 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -28616,6 +28646,62 @@
       <c r="Y1000" s="3"/>
       <c r="Z1000" s="3"/>
     </row>
+    <row r="1001">
+      <c r="A1001" s="3"/>
+      <c r="B1001" s="3"/>
+      <c r="C1001" s="3"/>
+      <c r="D1001" s="3"/>
+      <c r="E1001" s="3"/>
+      <c r="F1001" s="3"/>
+      <c r="G1001" s="3"/>
+      <c r="H1001" s="3"/>
+      <c r="I1001" s="3"/>
+      <c r="J1001" s="3"/>
+      <c r="K1001" s="3"/>
+      <c r="L1001" s="3"/>
+      <c r="M1001" s="3"/>
+      <c r="N1001" s="3"/>
+      <c r="O1001" s="3"/>
+      <c r="P1001" s="3"/>
+      <c r="Q1001" s="3"/>
+      <c r="R1001" s="3"/>
+      <c r="S1001" s="3"/>
+      <c r="T1001" s="3"/>
+      <c r="U1001" s="3"/>
+      <c r="V1001" s="3"/>
+      <c r="W1001" s="3"/>
+      <c r="X1001" s="3"/>
+      <c r="Y1001" s="3"/>
+      <c r="Z1001" s="3"/>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="3"/>
+      <c r="B1002" s="3"/>
+      <c r="C1002" s="3"/>
+      <c r="D1002" s="3"/>
+      <c r="E1002" s="3"/>
+      <c r="F1002" s="3"/>
+      <c r="G1002" s="3"/>
+      <c r="H1002" s="3"/>
+      <c r="I1002" s="3"/>
+      <c r="J1002" s="3"/>
+      <c r="K1002" s="3"/>
+      <c r="L1002" s="3"/>
+      <c r="M1002" s="3"/>
+      <c r="N1002" s="3"/>
+      <c r="O1002" s="3"/>
+      <c r="P1002" s="3"/>
+      <c r="Q1002" s="3"/>
+      <c r="R1002" s="3"/>
+      <c r="S1002" s="3"/>
+      <c r="T1002" s="3"/>
+      <c r="U1002" s="3"/>
+      <c r="V1002" s="3"/>
+      <c r="W1002" s="3"/>
+      <c r="X1002" s="3"/>
+      <c r="Y1002" s="3"/>
+      <c r="Z1002" s="3"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>